<commit_message>
avoid double ups in town_point's
</commit_message>
<xml_diff>
--- a/input/drive_times/Qld_towns_RSQ pathways V3.xlsx
+++ b/input/drive_times/Qld_towns_RSQ pathways V3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n10891277\R_projects\iTRAQI\input\drive_times\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA651B0C-B342-4B47-934C-15F4258CC625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE10BEB-9BE7-4DC6-9386-D0BB8E705EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="165" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Qld_towns (002)" sheetId="1" r:id="rId1"/>
@@ -289,7 +289,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4107" uniqueCount="1468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4107" uniqueCount="1472">
   <si>
     <t>Notes</t>
   </si>
@@ -4693,6 +4693,18 @@
   </si>
   <si>
     <t>STANTHORPE</t>
+  </si>
+  <si>
+    <t>TWP32601</t>
+  </si>
+  <si>
+    <t>TWN32601</t>
+  </si>
+  <si>
+    <t>TWP311601</t>
+  </si>
+  <si>
+    <t>TWN311601</t>
   </si>
 </sst>
 </file>
@@ -5697,10 +5709,10 @@
   <dimension ref="A1:AD444"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E389" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L442" sqref="L442"/>
+      <selection pane="bottomRight" activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21828,10 +21840,10 @@
     </row>
     <row r="216" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>696</v>
+        <v>1468</v>
       </c>
       <c r="B216" t="s">
-        <v>697</v>
+        <v>1469</v>
       </c>
       <c r="C216">
         <v>1</v>
@@ -27933,10 +27945,10 @@
     </row>
     <row r="304" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>394</v>
+        <v>1470</v>
       </c>
       <c r="B304" t="s">
-        <v>395</v>
+        <v>1471</v>
       </c>
       <c r="C304">
         <v>0</v>
@@ -37015,6 +37027,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D81C8DAA73B734408F5A245ECA39974D" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4cd869bab22379d10c014b7d810c789">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c4c4495c-ddbe-4376-9136-c67bc16b36da" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5c88b58a1626062d55ee341b4bde0044" ns2:_="">
     <xsd:import namespace="c4c4495c-ddbe-4376-9136-c67bc16b36da"/>
@@ -37198,12 +37216,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -37214,6 +37226,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6A3C46D-FEB1-451F-AC78-8B8706F2C3A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c4c4495c-ddbe-4376-9136-c67bc16b36da"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB20B413-81BC-4FB4-BEE8-0D613EFA2D83}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37231,22 +37259,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6A3C46D-FEB1-451F-AC78-8B8706F2C3A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c4c4495c-ddbe-4376-9136-c67bc16b36da"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5067268C-DEE0-42A6-B914-740AB6B9D34D}">
   <ds:schemaRefs>

</xml_diff>